<commit_message>
Add UI instructions for user marksheet
</commit_message>
<xml_diff>
--- a/TestData/BIOL5002 (2023011) Grades.xlsx
+++ b/TestData/BIOL5002 (2023011) Grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="84">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">CWS2WEEK12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quiz3</t>
   </si>
   <si>
     <t xml:space="preserve">Last downloaded from this course</t>
@@ -382,15 +385,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -412,800 +415,944 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="0" t="n">
+        <f aca="false">(G2*100)/100</f>
+        <v>57</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="0" t="n">
+        <f aca="false">(G3*100)/100</f>
+        <v>59</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="0" t="n">
+        <f aca="false">(G4*100)/100</f>
+        <v>58</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="0" t="n">
+        <f aca="false">(G5*100)/100</f>
+        <v>42</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H6" s="0" t="n">
+        <f aca="false">(G6*100)/100</f>
+        <v>52</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="0" t="n">
+        <f aca="false">(G7*100)/100</f>
+        <v>51</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="0" t="n">
+        <f aca="false">(G8*100)/100</f>
+        <v>81</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="0" t="n">
+        <f aca="false">(G9*100)/100</f>
+        <v>52</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="0" t="n">
+        <f aca="false">(G10*100)/100</f>
+        <v>52</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="0" t="n">
+        <f aca="false">(G11*100)/100</f>
+        <v>63</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H12" s="0" t="n">
+        <f aca="false">(G12*100)/100</f>
+        <v>64</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>62</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H13" s="0" t="n">
+        <f aca="false">(G13*100)/100</f>
+        <v>62</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H14" s="0" t="n">
+        <f aca="false">(G14*100)/100</f>
+        <v>65</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>61</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H15" s="0" t="n">
+        <f aca="false">(G15*100)/100</f>
+        <v>61</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H16" s="0" t="n">
+        <f aca="false">(G16*100)/100</f>
+        <v>67</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H17" s="0" t="n">
+        <f aca="false">(G17*100)/100</f>
+        <v>60</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H18" s="0" t="n">
+        <f aca="false">(G18*100)/100</f>
+        <v>53</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H19" s="0" t="n">
+        <f aca="false">(G19*100)/100</f>
+        <v>41</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H20" s="0" t="n">
+        <f aca="false">(G20*100)/100</f>
+        <v>65</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H23" s="0" t="n">
+        <f aca="false">(G23*100)/100</f>
+        <v>40</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H24" s="0" t="n">
+        <f aca="false">(G24*100)/100</f>
+        <v>59</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H25" s="0" t="n">
+        <f aca="false">(G25*100)/100</f>
+        <v>63</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H26" s="0" t="n">
+        <f aca="false">(G26*100)/100</f>
+        <v>63</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H28" s="0" t="n">
+        <f aca="false">(G28*100)/100</f>
+        <v>52</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H29" s="0" t="n">
+        <f aca="false">(G29*100)/100</f>
+        <v>65</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G30" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H30" s="0" t="n">
+        <f aca="false">(G30*100)/100</f>
+        <v>52</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G31" s="0" t="n">
         <v>69</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H31" s="0" t="n">
+        <f aca="false">(G31*100)/100</f>
+        <v>69</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H32" s="0" t="n">
+        <f aca="false">(G32*100)/100</f>
+        <v>59</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>62</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H33" s="0" t="n">
+        <f aca="false">(G33*100)/100</f>
+        <v>62</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H34" s="0" t="n">
+        <f aca="false">(G34*100)/100</f>
+        <v>46</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G35" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H35" s="0" t="n">
+        <f aca="false">(G35*100)/100</f>
+        <v>49</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G36" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H36" s="0" t="n">
+        <f aca="false">(G36*100)/100</f>
+        <v>55</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G37" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>11</v>
+      <c r="H37" s="0" t="n">
+        <f aca="false">(G37*100)/100</f>
+        <v>76</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>